<commit_message>
add minneapolis and rerun
</commit_message>
<xml_diff>
--- a/report/output/shr/clearance_demographics_New York.xlsx
+++ b/report/output/shr/clearance_demographics_New York.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\cmhacker\projects\homicide-clearance-fbi-data\report\output\shr\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D221380C-E009-4708-A2B9-FFBAACC38D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="NY" sheetId="1" r:id="rId1"/>
     <sheet name="NEW YORK CITY PD NEW YORK" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -68,11 +62,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,14 +130,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -190,7 +176,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -222,27 +208,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -274,24 +242,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -467,27 +417,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -516,7 +462,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1995</v>
       </c>
@@ -539,10 +485,10 @@
         <v>0.16</v>
       </c>
       <c r="I2" s="1">
-        <v>0.52173913043478259</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.5217391304347826</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>1996</v>
       </c>
@@ -550,25 +496,25 @@
         <v>9</v>
       </c>
       <c r="C3" s="1">
-        <v>0.45632530120481929</v>
+        <v>0.4563253012048193</v>
       </c>
       <c r="E3" s="1">
-        <v>0.42857142857142849</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="F3" s="1">
-        <v>0.82352941176470584</v>
+        <v>0.8235294117647058</v>
       </c>
       <c r="G3" s="1">
         <v>0.5</v>
       </c>
       <c r="H3" s="1">
-        <v>0.42857142857142849</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="I3" s="1">
-        <v>0.47952218430034121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.4795221843003412</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>1997</v>
       </c>
@@ -576,7 +522,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="1">
-        <v>0.48672566371681408</v>
+        <v>0.4867256637168141</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -594,7 +540,7 @@
         <v>0.5818965517241379</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>1998</v>
       </c>
@@ -602,22 +548,22 @@
         <v>9</v>
       </c>
       <c r="C5" s="1">
-        <v>0.52025586353944564</v>
+        <v>0.5202558635394456</v>
       </c>
       <c r="E5" s="1">
         <v>0.5</v>
       </c>
       <c r="F5" s="1">
-        <v>0.47058823529411759</v>
+        <v>0.4705882352941176</v>
       </c>
       <c r="H5" s="1">
-        <v>0.62068965517241381</v>
+        <v>0.6206896551724138</v>
       </c>
       <c r="I5" s="1">
-        <v>0.60621761658031093</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.6062176165803109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>1999</v>
       </c>
@@ -625,19 +571,19 @@
         <v>9</v>
       </c>
       <c r="C6" s="1">
-        <v>0.56673960612691465</v>
+        <v>0.5667396061269147</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
       </c>
       <c r="H6" s="1">
-        <v>0.36363636363636359</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="I6" s="1">
-        <v>0.58730158730158732</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.5873015873015873</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>2000</v>
       </c>
@@ -645,7 +591,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="1">
-        <v>0.53875968992248058</v>
+        <v>0.5387596899224806</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
@@ -654,13 +600,13 @@
         <v>0.5</v>
       </c>
       <c r="H7" s="1">
-        <v>0.44444444444444442</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="I7" s="1">
-        <v>0.64878048780487807</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.6487804878048781</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>2001</v>
       </c>
@@ -677,13 +623,13 @@
         <v>0.8</v>
       </c>
       <c r="H8" s="1">
-        <v>0.27272727272727271</v>
+        <v>0.2727272727272727</v>
       </c>
       <c r="I8" s="1">
         <v>0.6594594594594595</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>2002</v>
       </c>
@@ -691,7 +637,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="1">
-        <v>0.54671968190854869</v>
+        <v>0.5467196819085487</v>
       </c>
       <c r="E9" s="1">
         <v>0.5</v>
@@ -703,10 +649,10 @@
         <v>0.6785714285714286</v>
       </c>
       <c r="I9" s="1">
-        <v>0.69054441260744981</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.6905444126074498</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>2003</v>
       </c>
@@ -723,13 +669,13 @@
         <v>1</v>
       </c>
       <c r="H10" s="1">
-        <v>0.42857142857142849</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="I10" s="1">
-        <v>0.60571428571428576</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.6057142857142858</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>2004</v>
       </c>
@@ -737,7 +683,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="1">
-        <v>0.49486652977412732</v>
+        <v>0.4948665297741273</v>
       </c>
       <c r="F11" s="1">
         <v>0.5</v>
@@ -746,10 +692,10 @@
         <v>0.4</v>
       </c>
       <c r="I11" s="1">
-        <v>0.64082687338501287</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.6408268733850129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>2005</v>
       </c>
@@ -757,7 +703,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="1">
-        <v>0.50709939148073024</v>
+        <v>0.5070993914807302</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
@@ -766,13 +712,13 @@
         <v>1</v>
       </c>
       <c r="H12" s="1">
-        <v>0.58823529411764708</v>
+        <v>0.5882352941176471</v>
       </c>
       <c r="I12" s="1">
-        <v>0.62429378531073443</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.6242937853107344</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>2006</v>
       </c>
@@ -780,22 +726,22 @@
         <v>9</v>
       </c>
       <c r="C13" s="1">
-        <v>0.55353901996370236</v>
+        <v>0.5535390199637024</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
       </c>
       <c r="F13" s="1">
-        <v>0.53333333333333333</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="H13" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="I13" s="1">
-        <v>0.72677595628415304</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.726775956284153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>2007</v>
       </c>
@@ -803,7 +749,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="1">
-        <v>0.51716738197424894</v>
+        <v>0.5171673819742489</v>
       </c>
       <c r="D14" s="1">
         <v>0.6344827586206897</v>
@@ -815,10 +761,10 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="I14" s="1">
-        <v>0.83211678832116787</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.8321167883211679</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>2008</v>
       </c>
@@ -826,7 +772,7 @@
         <v>9</v>
       </c>
       <c r="C15" s="1">
-        <v>0.52277657266811284</v>
+        <v>0.5227765726681128</v>
       </c>
       <c r="D15" s="1">
         <v>0.660377358490566</v>
@@ -838,13 +784,13 @@
         <v>1</v>
       </c>
       <c r="H15" s="1">
-        <v>0.55172413793103448</v>
+        <v>0.5517241379310345</v>
       </c>
       <c r="I15" s="1">
-        <v>0.77160493827160492</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.7716049382716049</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>2009</v>
       </c>
@@ -852,16 +798,16 @@
         <v>9</v>
       </c>
       <c r="C16" s="1">
-        <v>0.54228855721393032</v>
+        <v>0.5422885572139303</v>
       </c>
       <c r="D16" s="1">
-        <v>0.60119047619047616</v>
+        <v>0.6011904761904762</v>
       </c>
       <c r="E16" s="1">
         <v>0.5</v>
       </c>
       <c r="F16" s="1">
-        <v>0.73684210526315785</v>
+        <v>0.7368421052631579</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
@@ -870,10 +816,10 @@
         <v>0.625</v>
       </c>
       <c r="I16" s="1">
-        <v>0.81159420289855078</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.8115942028985508</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>2010</v>
       </c>
@@ -881,25 +827,25 @@
         <v>9</v>
       </c>
       <c r="C17" s="1">
-        <v>0.51372549019607838</v>
+        <v>0.5137254901960784</v>
       </c>
       <c r="D17" s="1">
-        <v>0.65088757396449703</v>
+        <v>0.650887573964497</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
       </c>
       <c r="F17" s="1">
-        <v>0.78947368421052633</v>
+        <v>0.7894736842105263</v>
       </c>
       <c r="H17" s="1">
         <v>0.1666666666666666</v>
       </c>
       <c r="I17" s="1">
-        <v>0.73109243697478987</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.7310924369747899</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>2011</v>
       </c>
@@ -910,25 +856,25 @@
         <v>0.5717592592592593</v>
       </c>
       <c r="D18" s="1">
-        <v>0.62732919254658381</v>
+        <v>0.6273291925465838</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
       </c>
       <c r="F18" s="1">
-        <v>0.77777777777777779</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="G18" s="1">
         <v>1</v>
       </c>
       <c r="H18" s="1">
-        <v>0.55555555555555558</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="I18" s="1">
-        <v>0.80341880341880345</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.8034188034188035</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>2012</v>
       </c>
@@ -936,16 +882,16 @@
         <v>9</v>
       </c>
       <c r="C19" s="1">
-        <v>0.49357326478149099</v>
+        <v>0.493573264781491</v>
       </c>
       <c r="D19" s="1">
-        <v>0.60869565217391308</v>
+        <v>0.6086956521739131</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
       </c>
       <c r="F19" s="1">
-        <v>0.78947368421052633</v>
+        <v>0.7894736842105263</v>
       </c>
       <c r="G19" s="1">
         <v>1</v>
@@ -954,10 +900,10 @@
         <v>0.8</v>
       </c>
       <c r="I19" s="1">
-        <v>0.82692307692307687</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.8269230769230769</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>2013</v>
       </c>
@@ -965,16 +911,16 @@
         <v>9</v>
       </c>
       <c r="C20" s="1">
-        <v>0.52298850574712641</v>
+        <v>0.5229885057471264</v>
       </c>
       <c r="D20" s="1">
-        <v>0.71296296296296291</v>
+        <v>0.7129629629629629</v>
       </c>
       <c r="E20" s="1">
         <v>0.5</v>
       </c>
       <c r="F20" s="1">
-        <v>0.83333333333333337</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="G20" s="1">
         <v>1</v>
@@ -983,10 +929,10 @@
         <v>0.7857142857142857</v>
       </c>
       <c r="I20" s="1">
-        <v>0.85833333333333328</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.8583333333333333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>2014</v>
       </c>
@@ -997,22 +943,22 @@
         <v>0.5300546448087432</v>
       </c>
       <c r="D21" s="1">
-        <v>0.73451327433628322</v>
+        <v>0.7345132743362832</v>
       </c>
       <c r="F21" s="1">
-        <v>0.78947368421052633</v>
+        <v>0.7894736842105263</v>
       </c>
       <c r="G21" s="1">
         <v>1</v>
       </c>
       <c r="H21" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="I21" s="1">
         <v>0.8571428571428571</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>2015</v>
       </c>
@@ -1020,22 +966,22 @@
         <v>9</v>
       </c>
       <c r="C22" s="1">
-        <v>0.55890410958904113</v>
+        <v>0.5589041095890411</v>
       </c>
       <c r="D22" s="1">
-        <v>0.67741935483870963</v>
+        <v>0.6774193548387096</v>
       </c>
       <c r="F22" s="1">
-        <v>0.93333333333333324</v>
+        <v>0.9333333333333332</v>
       </c>
       <c r="H22" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="I22" s="1">
-        <v>0.87735849056603776</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.8773584905660378</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>2016</v>
       </c>
@@ -1043,10 +989,10 @@
         <v>9</v>
       </c>
       <c r="C23" s="1">
-        <v>0.54985754985754987</v>
+        <v>0.5498575498575499</v>
       </c>
       <c r="D23" s="1">
-        <v>0.75886524822695034</v>
+        <v>0.7588652482269503</v>
       </c>
       <c r="E23" s="1">
         <v>1</v>
@@ -1061,10 +1007,10 @@
         <v>0.4</v>
       </c>
       <c r="I23" s="1">
-        <v>0.90243902439024404</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.902439024390244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>2017</v>
       </c>
@@ -1075,13 +1021,13 @@
         <v>0.6512455516014235</v>
       </c>
       <c r="D24" s="1">
-        <v>0.69672131147540983</v>
+        <v>0.6967213114754098</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
       </c>
       <c r="F24" s="1">
-        <v>0.94444444444444442</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="G24" s="1">
         <v>1</v>
@@ -1090,10 +1036,10 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="I24" s="1">
-        <v>0.92523364485981319</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.9252336448598132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>2018</v>
       </c>
@@ -1101,28 +1047,28 @@
         <v>9</v>
       </c>
       <c r="C25" s="1">
-        <v>0.58085808580858089</v>
+        <v>0.5808580858085809</v>
       </c>
       <c r="D25" s="1">
-        <v>0.79047619047619044</v>
+        <v>0.7904761904761904</v>
       </c>
       <c r="E25" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F25" s="1">
-        <v>0.90909090909090917</v>
+        <v>0.9090909090909092</v>
       </c>
       <c r="G25" s="1">
         <v>1</v>
       </c>
       <c r="H25" s="1">
-        <v>0.73333333333333328</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="I25" s="1">
         <v>0.84</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>2019</v>
       </c>
@@ -1130,25 +1076,25 @@
         <v>9</v>
       </c>
       <c r="C26" s="1">
-        <v>0.60389610389610393</v>
+        <v>0.6038961038961039</v>
       </c>
       <c r="D26" s="1">
-        <v>0.69747899159663862</v>
+        <v>0.6974789915966386</v>
       </c>
       <c r="E26" s="1">
         <v>0.8</v>
       </c>
       <c r="F26" s="1">
-        <v>0.72727272727272729</v>
+        <v>0.7272727272727273</v>
       </c>
       <c r="H26" s="1">
-        <v>0.83333333333333337</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="I26" s="1">
-        <v>0.89873417721518989</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.8987341772151899</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>2020</v>
       </c>
@@ -1156,22 +1102,22 @@
         <v>9</v>
       </c>
       <c r="C27" s="1">
-        <v>0.53360488798370675</v>
+        <v>0.5336048879837068</v>
       </c>
       <c r="D27" s="1">
-        <v>0.61176470588235299</v>
+        <v>0.611764705882353</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
       </c>
       <c r="F27" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="H27" s="1">
         <v>0.25</v>
       </c>
       <c r="I27" s="1">
-        <v>0.84615384615384615</v>
+        <v>0.8461538461538461</v>
       </c>
     </row>
   </sheetData>
@@ -1180,24 +1126,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="18.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="23.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1229,7 +1175,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1995</v>
       </c>
@@ -1240,25 +1186,25 @@
         <v>13</v>
       </c>
       <c r="D2" s="1">
-        <v>0.45439469320066328</v>
+        <v>0.4543946932006633</v>
       </c>
       <c r="F2" s="1">
         <v>0.5</v>
       </c>
       <c r="G2" s="1">
-        <v>0.36363636363636359</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="H2" s="1">
         <v>1</v>
       </c>
       <c r="I2" s="1">
-        <v>9.5238095238095205E-2</v>
+        <v>0.09523809523809521</v>
       </c>
       <c r="J2" s="1">
         <v>0.4575289575289575</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>1996</v>
       </c>
@@ -1269,25 +1215,25 @@
         <v>13</v>
       </c>
       <c r="D3" s="1">
-        <v>0.43712574850299402</v>
+        <v>0.437125748502994</v>
       </c>
       <c r="F3" s="1">
-        <v>0.42857142857142849</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="G3" s="1">
-        <v>0.90909090909090917</v>
+        <v>0.9090909090909092</v>
       </c>
       <c r="H3" s="1">
         <v>0.5</v>
       </c>
       <c r="I3" s="1">
-        <v>0.46153846153846151</v>
+        <v>0.4615384615384615</v>
       </c>
       <c r="J3" s="1">
-        <v>0.40224719101123591</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.4022471910112359</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>1997</v>
       </c>
@@ -1298,22 +1244,22 @@
         <v>13</v>
       </c>
       <c r="D4" s="1">
-        <v>0.46394230769230771</v>
+        <v>0.4639423076923077</v>
       </c>
       <c r="G4" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <v>0.70370370370370372</v>
+        <v>0.7037037037037037</v>
       </c>
       <c r="J4" s="1">
-        <v>0.52279635258358659</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.5227963525835866</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>1998</v>
       </c>
@@ -1324,7 +1270,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="1">
-        <v>0.49147727272727271</v>
+        <v>0.4914772727272727</v>
       </c>
       <c r="F5" s="1">
         <v>0.5</v>
@@ -1336,10 +1282,10 @@
         <v>0.64</v>
       </c>
       <c r="J5" s="1">
-        <v>0.52059925093632964</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.5205992509363296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>1999</v>
       </c>
@@ -1350,16 +1296,16 @@
         <v>13</v>
       </c>
       <c r="D6" s="1">
-        <v>0.53424657534246578</v>
+        <v>0.5342465753424658</v>
       </c>
       <c r="I6" s="1">
         <v>0.25</v>
       </c>
       <c r="J6" s="1">
-        <v>0.50974025974025972</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.5097402597402597</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>2000</v>
       </c>
@@ -1370,16 +1316,16 @@
         <v>13</v>
       </c>
       <c r="D7" s="1">
-        <v>0.53589743589743588</v>
+        <v>0.5358974358974359</v>
       </c>
       <c r="I7" s="1">
         <v>0.2857142857142857</v>
       </c>
       <c r="J7" s="1">
-        <v>0.58389261744966447</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.5838926174496645</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>2001</v>
       </c>
@@ -1390,7 +1336,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="1">
-        <v>0.60309278350515461</v>
+        <v>0.6030927835051546</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
@@ -1402,7 +1348,7 @@
         <v>0.6045627376425855</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>2002</v>
       </c>
@@ -1419,10 +1365,10 @@
         <v>0.65</v>
       </c>
       <c r="J9" s="1">
-        <v>0.64224137931034486</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.6422413793103449</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>2003</v>
       </c>
@@ -1442,10 +1388,10 @@
         <v>0.2</v>
       </c>
       <c r="J10" s="1">
-        <v>0.53138075313807531</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.5313807531380753</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>2004</v>
       </c>
@@ -1456,16 +1402,16 @@
         <v>13</v>
       </c>
       <c r="D11" s="1">
-        <v>0.47976878612716761</v>
+        <v>0.4797687861271676</v>
       </c>
       <c r="I11" s="1">
         <v>0</v>
       </c>
       <c r="J11" s="1">
-        <v>0.56611570247933884</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.5661157024793388</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>2005</v>
       </c>
@@ -1476,7 +1422,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="1">
-        <v>0.48159509202453987</v>
+        <v>0.4815950920245399</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -1485,10 +1431,10 @@
         <v>0.5714285714285714</v>
       </c>
       <c r="J12" s="1">
-        <v>0.50724637681159424</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.5072463768115942</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>2006</v>
       </c>
@@ -1499,19 +1445,19 @@
         <v>13</v>
       </c>
       <c r="D13" s="1">
-        <v>0.61025641025641031</v>
+        <v>0.6102564102564103</v>
       </c>
       <c r="G13" s="1">
-        <v>0.53333333333333333</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="I13" s="1">
         <v>0</v>
       </c>
       <c r="J13" s="1">
-        <v>0.70192307692307687</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.7019230769230769</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>2007</v>
       </c>
@@ -1522,10 +1468,10 @@
         <v>13</v>
       </c>
       <c r="D14" s="1">
-        <v>0.53674121405750796</v>
+        <v>0.536741214057508</v>
       </c>
       <c r="E14" s="1">
-        <v>0.64864864864864868</v>
+        <v>0.6486486486486487</v>
       </c>
       <c r="G14" s="1">
         <v>0.7</v>
@@ -1534,10 +1480,10 @@
         <v>0.5</v>
       </c>
       <c r="J14" s="1">
-        <v>0.86363636363636365</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.8636363636363636</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>2008</v>
       </c>
@@ -1548,19 +1494,19 @@
         <v>13</v>
       </c>
       <c r="D15" s="1">
-        <v>0.54716981132075471</v>
+        <v>0.5471698113207547</v>
       </c>
       <c r="E15" s="1">
-        <v>0.66949152542372881</v>
+        <v>0.6694915254237288</v>
       </c>
       <c r="I15" s="1">
-        <v>0.53846153846153844</v>
+        <v>0.5384615384615384</v>
       </c>
       <c r="J15" s="1">
-        <v>0.76363636363636367</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.7636363636363637</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>2009</v>
       </c>
@@ -1571,7 +1517,7 @@
         <v>13</v>
       </c>
       <c r="D16" s="1">
-        <v>0.53787878787878785</v>
+        <v>0.5378787878787878</v>
       </c>
       <c r="E16" s="1">
         <v>0.65</v>
@@ -1580,16 +1526,16 @@
         <v>1</v>
       </c>
       <c r="G16" s="1">
-        <v>0.70588235294117652</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="I16" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="J16" s="1">
         <v>0.6470588235294118</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>2010</v>
       </c>
@@ -1600,16 +1546,16 @@
         <v>13</v>
       </c>
       <c r="D17" s="1">
-        <v>0.48245614035087719</v>
+        <v>0.4824561403508772</v>
       </c>
       <c r="E17" s="1">
-        <v>0.61016949152542377</v>
+        <v>0.6101694915254238</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
       </c>
       <c r="G17" s="1">
-        <v>0.77777777777777779</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="I17" s="1">
         <v>0</v>
@@ -1618,7 +1564,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>2011</v>
       </c>
@@ -1629,10 +1575,10 @@
         <v>13</v>
       </c>
       <c r="D18" s="1">
-        <v>0.55205047318611988</v>
+        <v>0.5520504731861199</v>
       </c>
       <c r="E18" s="1">
-        <v>0.60317460317460314</v>
+        <v>0.6031746031746031</v>
       </c>
       <c r="G18" s="1">
         <v>0.8125</v>
@@ -1647,7 +1593,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>2012</v>
       </c>
@@ -1658,22 +1604,22 @@
         <v>13</v>
       </c>
       <c r="D19" s="1">
-        <v>0.51821862348178138</v>
+        <v>0.5182186234817814</v>
       </c>
       <c r="E19" s="1">
-        <v>0.63725490196078427</v>
+        <v>0.6372549019607843</v>
       </c>
       <c r="G19" s="1">
-        <v>0.76470588235294112</v>
+        <v>0.7647058823529411</v>
       </c>
       <c r="I19" s="1">
         <v>1</v>
       </c>
       <c r="J19" s="1">
-        <v>0.75609756097560976</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.7560975609756098</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>2013</v>
       </c>
@@ -1684,25 +1630,25 @@
         <v>13</v>
       </c>
       <c r="D20" s="1">
-        <v>0.55665024630541871</v>
+        <v>0.5566502463054187</v>
       </c>
       <c r="E20" s="1">
-        <v>0.74358974358974361</v>
+        <v>0.7435897435897436</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
       </c>
       <c r="G20" s="1">
-        <v>0.76923076923076927</v>
+        <v>0.7692307692307693</v>
       </c>
       <c r="I20" s="1">
         <v>1</v>
       </c>
       <c r="J20" s="1">
-        <v>0.82608695652173914</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.8260869565217391</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>2014</v>
       </c>
@@ -1713,13 +1659,13 @@
         <v>13</v>
       </c>
       <c r="D21" s="1">
-        <v>0.53588516746411485</v>
+        <v>0.5358851674641149</v>
       </c>
       <c r="E21" s="1">
-        <v>0.80769230769230771</v>
+        <v>0.8076923076923077</v>
       </c>
       <c r="G21" s="1">
-        <v>0.88235294117647056</v>
+        <v>0.8823529411764706</v>
       </c>
       <c r="H21" s="1">
         <v>1</v>
@@ -1728,7 +1674,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>2015</v>
       </c>
@@ -1739,22 +1685,22 @@
         <v>13</v>
       </c>
       <c r="D22" s="1">
-        <v>0.54222222222222227</v>
+        <v>0.5422222222222223</v>
       </c>
       <c r="E22" s="1">
-        <v>0.66304347826086951</v>
+        <v>0.6630434782608695</v>
       </c>
       <c r="G22" s="1">
         <v>0.9</v>
       </c>
       <c r="I22" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="J22" s="1">
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>2016</v>
       </c>
@@ -1765,7 +1711,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="1">
-        <v>0.56218905472636815</v>
+        <v>0.5621890547263682</v>
       </c>
       <c r="E23" s="1">
         <v>0.8125</v>
@@ -1780,7 +1726,7 @@
         <v>0.8571428571428571</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>2017</v>
       </c>
@@ -1791,13 +1737,13 @@
         <v>13</v>
       </c>
       <c r="D24" s="1">
-        <v>0.73584905660377353</v>
+        <v>0.7358490566037735</v>
       </c>
       <c r="E24" s="1">
-        <v>0.73809523809523814</v>
+        <v>0.7380952380952381</v>
       </c>
       <c r="G24" s="1">
-        <v>0.93333333333333324</v>
+        <v>0.9333333333333332</v>
       </c>
       <c r="I24" s="1">
         <v>1</v>
@@ -1806,7 +1752,7 @@
         <v>0.9629629629629628</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>2018</v>
       </c>
@@ -1817,25 +1763,25 @@
         <v>13</v>
       </c>
       <c r="D25" s="1">
-        <v>0.67613636363636365</v>
+        <v>0.6761363636363636</v>
       </c>
       <c r="E25" s="1">
-        <v>0.81428571428571428</v>
+        <v>0.8142857142857143</v>
       </c>
       <c r="F25" s="1">
         <v>1</v>
       </c>
       <c r="G25" s="1">
-        <v>0.90909090909090917</v>
+        <v>0.9090909090909092</v>
       </c>
       <c r="I25" s="1">
         <v>0.75</v>
       </c>
       <c r="J25" s="1">
-        <v>0.78260869565217395</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.7826086956521739</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>2019</v>
       </c>
@@ -1846,10 +1792,10 @@
         <v>13</v>
       </c>
       <c r="D26" s="1">
-        <v>0.69318181818181823</v>
+        <v>0.6931818181818182</v>
       </c>
       <c r="E26" s="1">
-        <v>0.71590909090909094</v>
+        <v>0.7159090909090909</v>
       </c>
       <c r="F26" s="1">
         <v>1</v>
@@ -1861,10 +1807,10 @@
         <v>0.8</v>
       </c>
       <c r="J26" s="1">
-        <v>0.93333333333333324</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.9333333333333332</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>2020</v>
       </c>
@@ -1875,19 +1821,19 @@
         <v>13</v>
       </c>
       <c r="D27" s="1">
-        <v>0.56622516556291391</v>
+        <v>0.5662251655629139</v>
       </c>
       <c r="E27" s="1">
-        <v>0.65573770491803274</v>
+        <v>0.6557377049180327</v>
       </c>
       <c r="G27" s="1">
-        <v>0.63636363636363635</v>
+        <v>0.6363636363636364</v>
       </c>
       <c r="I27" s="1">
         <v>0</v>
       </c>
       <c r="J27" s="1">
-        <v>0.82758620689655171</v>
+        <v>0.8275862068965517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>